<commit_message>
Updated decision support rules spreadsheet so that identification of overlapping rules by OWL reasoner can be shown in an even nicer way.
</commit_message>
<xml_diff>
--- a/knowledge-base/trunk/data/decision-support-rules/Pharmacogenomics decision support spreadsheet.xlsx
+++ b/knowledge-base/trunk/data/decision-support-rules/Pharmacogenomics decision support spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="630" windowWidth="10215" windowHeight="4755" activeTab="1"/>
+    <workbookView xWindow="270" yWindow="630" windowWidth="10215" windowHeight="4755"/>
   </bookViews>
   <sheets>
     <sheet name="CDS rules" sheetId="1" r:id="rId1"/>
@@ -755,12 +755,6 @@
 http://www.ncbi.nlm.nih.gov/pubmed/21412233</t>
   </si>
   <si>
-    <t>has exactly 2 (TPMT_star_2 or TPMT_star_3A or TPMT_star_3B or TPMT_star_3C or TPMT_star_4 or TPMT_star_5 or TPMT_star_6 or TPMT_star_7 or TPMT_star_8 or TPMT_star_9 or TPMT_star_10 or TPMT_star_11 or TPMT_star_12 or TPMT_star_13 or TPMT_star_14 or TPMT_star_15 or TPMT_star_16 or TPMT_star_17 or TPMT_star_18)</t>
-  </si>
-  <si>
-    <t>has some TPMT_star_1 and has some (TPMT_star_2 or TPMT_star_3A or TPMT_star_3B or TPMT_star_3C or TPMT_star_4 or TPMT_star_5 or TPMT_star_6 or TPMT_star_7 or TPMT_star_8 or TPMT_star_9 or TPMT_star_10 or TPMT_star_11 or TPMT_star_12 or TPMT_star_13 or TPMT_star_14 or TPMT_star_15 or TPMT_star_16 or TPMT_star_17 or TPMT_star_18)</t>
-  </si>
-  <si>
     <t>has exactly 2 (CYP2C19_star_1 or CYP2C19_star_17)</t>
   </si>
   <si>
@@ -856,6 +850,12 @@
   </si>
   <si>
     <t>An anticoagulant that acts by inhibiting the synthesis of vitamin K-dependent coagulation factors. Warfarin is indicated for the prophylaxis and/or treatment of venous thrombosis and its extension, pulmonary embolism, and atrial fibrillation with embolization. It is also used as an adjunct in the prophylaxis of systemic embolism after myocardial infarction. Warfarin is also used as a rodenticide. [Adapted from PubChem and DrugBank]</t>
+  </si>
+  <si>
+    <t>has some TPMT_star_1 and has some (TPMT_star_2 or TPMT_star_3 or TPMT_star_4 or TPMT_star_5 or TPMT_star_6 or TPMT_star_7 or TPMT_star_8 or TPMT_star_9 or TPMT_star_10 or TPMT_star_11 or TPMT_star_12 or TPMT_star_13 or TPMT_star_14 or TPMT_star_15 or TPMT_star_16 or TPMT_star_17 or TPMT_star_18)</t>
+  </si>
+  <si>
+    <t>has exactly 2 (TPMT_star_2 or TPMT_star_3A or TPMT_star_3 or TPMT_star_4 or TPMT_star_5 or TPMT_star_6 or TPMT_star_7 or TPMT_star_8 or TPMT_star_9 or TPMT_star_10 or TPMT_star_11 or TPMT_star_12 or TPMT_star_13 or TPMT_star_14 or TPMT_star_15 or TPMT_star_16 or TPMT_star_17 or TPMT_star_18)</t>
   </si>
 </sst>
 </file>
@@ -1519,7 +1519,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -1650,9 +1650,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1690,7 +1690,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1762,7 +1762,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1938,12 +1938,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R234"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="76.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="76.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.42578125" style="16" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" style="16" customWidth="1"/>
@@ -1966,7 +1966,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B1" s="33" t="s">
         <v>0</v>
@@ -1978,13 +1978,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="63" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F1" s="62" t="s">
+        <v>236</v>
+      </c>
+      <c r="G1" s="41" t="s">
         <v>238</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>240</v>
       </c>
       <c r="H1" s="42" t="s">
         <v>3</v>
@@ -2866,7 +2866,7 @@
         <v>56</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G20" s="22" t="s">
         <v>57</v>
@@ -2905,7 +2905,7 @@
         <v>60</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G21" s="23" t="s">
         <v>61</v>
@@ -2944,7 +2944,7 @@
         <v>63</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G22" s="53" t="s">
         <v>61</v>
@@ -2983,10 +2983,10 @@
         <v>65</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G23" s="60" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="K23" s="48" t="s">
         <v>66</v>
@@ -3025,10 +3025,10 @@
         <v>69</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G24" s="60" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K24" s="48" t="s">
         <v>66</v>
@@ -3067,10 +3067,10 @@
         <v>70</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G25" s="61" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="K25" s="51" t="s">
         <v>66</v>
@@ -3454,7 +3454,7 @@
         <v>86</v>
       </c>
       <c r="F35" s="29" t="s">
-        <v>229</v>
+        <v>259</v>
       </c>
       <c r="G35" s="23" t="s">
         <v>87</v>
@@ -3496,7 +3496,7 @@
         <v>91</v>
       </c>
       <c r="F36" s="29" t="s">
-        <v>228</v>
+        <v>260</v>
       </c>
       <c r="G36" s="53" t="s">
         <v>92</v>
@@ -3538,7 +3538,7 @@
         <v>86</v>
       </c>
       <c r="F37" s="29" t="s">
-        <v>229</v>
+        <v>259</v>
       </c>
       <c r="G37" s="23" t="s">
         <v>87</v>
@@ -3580,7 +3580,7 @@
         <v>91</v>
       </c>
       <c r="F38" s="29" t="s">
-        <v>228</v>
+        <v>260</v>
       </c>
       <c r="G38" s="53" t="s">
         <v>92</v>
@@ -3622,7 +3622,7 @@
         <v>224</v>
       </c>
       <c r="F39" s="29" t="s">
-        <v>229</v>
+        <v>259</v>
       </c>
       <c r="G39" s="23" t="s">
         <v>94</v>
@@ -3664,7 +3664,7 @@
         <v>225</v>
       </c>
       <c r="F40" s="29" t="s">
-        <v>228</v>
+        <v>260</v>
       </c>
       <c r="G40" s="49" t="s">
         <v>94</v>
@@ -3967,7 +3967,7 @@
         <v>121</v>
       </c>
       <c r="F48" s="29" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G48" s="22" t="s">
         <v>122</v>
@@ -4009,7 +4009,7 @@
         <v>124</v>
       </c>
       <c r="F49" s="29" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G49" s="23" t="s">
         <v>125</v>
@@ -4051,7 +4051,7 @@
         <v>126</v>
       </c>
       <c r="F50" s="29" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G50" s="46" t="s">
         <v>127</v>
@@ -8814,11 +8814,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="42.7109375" customWidth="1"/>
     <col min="3" max="3" width="63" customWidth="1"/>
@@ -8826,13 +8826,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="64" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="65" t="s">
         <v>246</v>
       </c>
-      <c r="B1" s="65" t="s">
-        <v>248</v>
-      </c>
       <c r="C1" s="12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8840,21 +8840,21 @@
         <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C2" s="67" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="89.25" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C3" s="66" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="89.25" x14ac:dyDescent="0.2">
@@ -8862,10 +8862,10 @@
         <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C4" s="67" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="114.75" x14ac:dyDescent="0.2">
@@ -8873,10 +8873,10 @@
         <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C5" s="67" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -8884,10 +8884,10 @@
         <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C6" s="67" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="127.5" x14ac:dyDescent="0.2">
@@ -8895,10 +8895,10 @@
         <v>15</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -8923,7 +8923,7 @@
       <selection pane="bottomLeft" activeCell="C1" sqref="C1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="32" customWidth="1"/>
     <col min="12" max="12" width="53.5703125" customWidth="1"/>

</xml_diff>

<commit_message>
Updated decision support spreadsheet with final version sent by Kathrin
</commit_message>
<xml_diff>
--- a/knowledge-base/trunk/data/decision-support-rules/Pharmacogenomics decision support spreadsheet.xlsx
+++ b/knowledge-base/trunk/data/decision-support-rules/Pharmacogenomics decision support spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="276" yWindow="636" windowWidth="10212" windowHeight="2688" activeTab="3"/>
+    <workbookView xWindow="276" yWindow="636" windowWidth="10212" windowHeight="2688"/>
   </bookViews>
   <sheets>
     <sheet name="CDS rules" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3463" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3473" uniqueCount="746">
   <si>
     <t>Rule status</t>
   </si>
@@ -2422,6 +2422,22 @@
   </si>
   <si>
     <t>has exactly 2 (CYP2D6_star_9 or CYP2D6_star_10 or CYP2D6_star_17 or CYP2D6_star_29 or CYP2D6_star_36 or CYP2D6_star_41) or has some (CYP2D6_star_1 or CYP2D6_star_2 or CYP2D6_star_33 or CYP2D6_star_35 or CYP2D6_star_9 or CYP2D6_star_10 or CYP2D6_star_17 or CYP2D6_star_29 or CYP2D6_star_36 or CYP2D6_star_41) and has some (CYP2D6_star_3 or CYP2D6_star_4 or CYP2D6_star_5 or CYP2D6_star_6 or CYP2D6_star_7 or CYP2D6_star_8 or CYP2D6_star_11 or CYP2D6_star_12 or CYP2D6_star_13 or CYP2D6_star_14 or CYP2D6_star_15 or CYP2D6_star_16 or CYP2D6_star_19 or CYP2D6_star_20 or CYP2D6_star_21 or CYP2D6_star_38 or CYP2D6_star_40 or CYP2D6_star_42)</t>
+  </si>
+  <si>
+    <t>The best way to estimate the anticipated stable dose of warfarin is to use the algorithms available on http://www.warfarindosing.org </t>
+  </si>
+  <si>
+    <t>http://www.pharmgkb.org/guideline/PA166104949
+http://www.pharmgkb.org/download.action?filename=Warfarin_CPIC_guidelines.pdf</t>
+  </si>
+  <si>
+    <t>Guideline applies exclusively to individuals of Korean descent with CDK stage 3 or worse or individuals of Han Chinese or Thai descent.</t>
+  </si>
+  <si>
+    <t>ad recommendation: This dosing recommendation applies to adults only.</t>
+  </si>
+  <si>
+    <t>Adult patients undergoing warfarin anticoagulant therapy</t>
   </si>
 </sst>
 </file>
@@ -3614,11 +3630,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:T299"/>
+  <dimension ref="A1:T300"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D302" sqref="D302"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S300" sqref="S300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.109375" defaultRowHeight="76.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15879,7 +15895,7 @@
     </row>
     <row r="254" spans="1:20" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="19" t="str">
-        <f t="shared" ref="A254:A299" si="4">"human triggering CDS rule " &amp; (ROW() - 1)</f>
+        <f t="shared" ref="A254:A300" si="4">"human triggering CDS rule " &amp; (ROW() - 1)</f>
         <v>human triggering CDS rule 253</v>
       </c>
       <c r="B254" s="22" t="s">
@@ -18016,6 +18032,9 @@
       <c r="H299" s="62" t="s">
         <v>735</v>
       </c>
+      <c r="I299" s="68" t="s">
+        <v>743</v>
+      </c>
       <c r="L299" s="74" t="s">
         <v>732</v>
       </c>
@@ -18030,10 +18049,54 @@
         <v>41592</v>
       </c>
       <c r="R299" s="70">
-        <v>41592</v>
+        <v>41597</v>
       </c>
       <c r="S299" s="71"/>
       <c r="T299" s="72" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="300" spans="1:20" s="68" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="67" t="str">
+        <f t="shared" si="4"/>
+        <v>human triggering CDS rule 299</v>
+      </c>
+      <c r="B300" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="C300" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="D300" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="E300" s="71" t="s">
+        <v>745</v>
+      </c>
+      <c r="F300" s="71"/>
+      <c r="H300" s="62" t="s">
+        <v>741</v>
+      </c>
+      <c r="I300" s="68" t="s">
+        <v>744</v>
+      </c>
+      <c r="L300" s="74" t="s">
+        <v>742</v>
+      </c>
+      <c r="O300" s="71" t="s">
+        <v>54</v>
+      </c>
+      <c r="P300" s="58">
+        <v>40793</v>
+      </c>
+      <c r="Q300" s="70">
+        <v>41594</v>
+      </c>
+      <c r="R300" s="70">
+        <v>41597</v>
+      </c>
+      <c r="S300" s="71"/>
+      <c r="T300" s="72" t="s">
         <v>219</v>
       </c>
     </row>
@@ -20760,8 +20823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K925"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>

</xml_diff>